<commit_message>
Removed unused code, updated .gitignore
</commit_message>
<xml_diff>
--- a/Excel/data.xlsx
+++ b/Excel/data.xlsx
@@ -840,7 +840,7 @@
         </is>
       </c>
       <c r="O7" t="n">
-        <v>181</v>
+        <v>235</v>
       </c>
       <c r="P7" t="inlineStr">
         <is>
@@ -906,7 +906,7 @@
         </is>
       </c>
       <c r="O8" t="n">
-        <v>33</v>
+        <v>57</v>
       </c>
       <c r="P8" t="inlineStr">
         <is>
@@ -972,7 +972,7 @@
         </is>
       </c>
       <c r="O9" t="n">
-        <v>301</v>
+        <v>258</v>
       </c>
       <c r="P9" t="inlineStr">
         <is>
@@ -1038,7 +1038,7 @@
         </is>
       </c>
       <c r="O10" t="n">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="P10" t="inlineStr">
         <is>
@@ -1104,7 +1104,7 @@
         </is>
       </c>
       <c r="O11" t="n">
-        <v>723</v>
+        <v>728</v>
       </c>
       <c r="P11" t="inlineStr">
         <is>
@@ -1170,7 +1170,7 @@
         </is>
       </c>
       <c r="O12" t="n">
-        <v>885</v>
+        <v>940</v>
       </c>
       <c r="P12" t="inlineStr">
         <is>
@@ -1236,7 +1236,7 @@
         </is>
       </c>
       <c r="O13" t="n">
-        <v>446</v>
+        <v>558</v>
       </c>
       <c r="P13" t="inlineStr">
         <is>
@@ -1302,7 +1302,7 @@
         </is>
       </c>
       <c r="O14" t="n">
-        <v>773</v>
+        <v>740</v>
       </c>
       <c r="P14" t="inlineStr">
         <is>
@@ -1368,7 +1368,7 @@
         </is>
       </c>
       <c r="O15" t="n">
-        <v>672</v>
+        <v>629</v>
       </c>
       <c r="P15" t="inlineStr">
         <is>
@@ -1434,7 +1434,7 @@
         </is>
       </c>
       <c r="O16" t="n">
-        <v>387</v>
+        <v>367</v>
       </c>
       <c r="P16" t="inlineStr">
         <is>
@@ -1500,7 +1500,7 @@
         </is>
       </c>
       <c r="O17" t="n">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="P17" t="inlineStr">
         <is>
@@ -1566,7 +1566,7 @@
         </is>
       </c>
       <c r="O18" t="n">
-        <v>192</v>
+        <v>175</v>
       </c>
       <c r="P18" t="inlineStr">
         <is>
@@ -1632,7 +1632,7 @@
         </is>
       </c>
       <c r="O19" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="P19" t="inlineStr">
         <is>
@@ -1698,7 +1698,7 @@
         </is>
       </c>
       <c r="O20" t="n">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="P20" t="inlineStr">
         <is>
@@ -1764,7 +1764,7 @@
         </is>
       </c>
       <c r="O21" t="n">
-        <v>139</v>
+        <v>154</v>
       </c>
       <c r="P21" t="inlineStr">
         <is>
@@ -1830,7 +1830,7 @@
         </is>
       </c>
       <c r="O22" t="n">
-        <v>349</v>
+        <v>360</v>
       </c>
       <c r="P22" t="inlineStr">
         <is>
@@ -1896,7 +1896,7 @@
         </is>
       </c>
       <c r="O23" t="n">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="P23" t="inlineStr">
         <is>
@@ -1962,7 +1962,7 @@
         </is>
       </c>
       <c r="O24" t="n">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="P24" t="inlineStr">
         <is>
@@ -2028,7 +2028,7 @@
         </is>
       </c>
       <c r="O25" t="n">
-        <v>398</v>
+        <v>458</v>
       </c>
       <c r="P25" t="inlineStr">
         <is>
@@ -2094,7 +2094,7 @@
         </is>
       </c>
       <c r="O26" t="n">
-        <v>394</v>
+        <v>467</v>
       </c>
       <c r="P26" t="inlineStr">
         <is>
@@ -2160,7 +2160,7 @@
         </is>
       </c>
       <c r="O27" t="n">
-        <v>111</v>
+        <v>98</v>
       </c>
       <c r="P27" t="inlineStr">
         <is>
@@ -2226,7 +2226,7 @@
         </is>
       </c>
       <c r="O28" t="n">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="P28" t="inlineStr">
         <is>
@@ -2292,7 +2292,7 @@
         </is>
       </c>
       <c r="O29" t="n">
-        <v>631</v>
+        <v>700</v>
       </c>
       <c r="P29" t="inlineStr">
         <is>
@@ -2358,7 +2358,7 @@
         </is>
       </c>
       <c r="O30" t="n">
-        <v>576</v>
+        <v>515</v>
       </c>
       <c r="P30" t="inlineStr">
         <is>
@@ -2424,7 +2424,7 @@
         </is>
       </c>
       <c r="O31" t="n">
-        <v>608</v>
+        <v>697</v>
       </c>
       <c r="P31" t="inlineStr">
         <is>
@@ -2490,7 +2490,7 @@
         </is>
       </c>
       <c r="O32" t="n">
-        <v>578</v>
+        <v>602</v>
       </c>
       <c r="P32" t="inlineStr">
         <is>
@@ -2556,7 +2556,7 @@
         </is>
       </c>
       <c r="O33" t="n">
-        <v>92</v>
+        <v>105</v>
       </c>
       <c r="P33" t="inlineStr">
         <is>
@@ -2622,7 +2622,7 @@
         </is>
       </c>
       <c r="O34" t="n">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="P34" t="inlineStr">
         <is>
@@ -2688,7 +2688,7 @@
         </is>
       </c>
       <c r="O35" t="n">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="P35" t="inlineStr">
         <is>
@@ -2754,7 +2754,7 @@
         </is>
       </c>
       <c r="O36" t="n">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="P36" t="inlineStr">
         <is>
@@ -2820,7 +2820,7 @@
         </is>
       </c>
       <c r="O37" t="n">
-        <v>590</v>
+        <v>548</v>
       </c>
       <c r="P37" t="inlineStr">
         <is>
@@ -2886,7 +2886,7 @@
         </is>
       </c>
       <c r="O38" t="n">
-        <v>318</v>
+        <v>343</v>
       </c>
       <c r="P38" t="inlineStr">
         <is>
@@ -2952,7 +2952,7 @@
         </is>
       </c>
       <c r="O39" t="n">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="P39" t="inlineStr">
         <is>
@@ -3018,7 +3018,7 @@
         </is>
       </c>
       <c r="O40" t="n">
-        <v>159</v>
+        <v>172</v>
       </c>
       <c r="P40" t="inlineStr">
         <is>
@@ -3084,7 +3084,7 @@
         </is>
       </c>
       <c r="O41" t="n">
-        <v>307</v>
+        <v>402</v>
       </c>
       <c r="P41" t="inlineStr">
         <is>
@@ -3150,7 +3150,7 @@
         </is>
       </c>
       <c r="O42" t="n">
-        <v>271</v>
+        <v>342</v>
       </c>
       <c r="P42" t="inlineStr">
         <is>
@@ -3216,7 +3216,7 @@
         </is>
       </c>
       <c r="O43" t="n">
-        <v>1060</v>
+        <v>961</v>
       </c>
       <c r="P43" t="inlineStr">
         <is>
@@ -3282,7 +3282,7 @@
         </is>
       </c>
       <c r="O44" t="n">
-        <v>1400</v>
+        <v>1108</v>
       </c>
       <c r="P44" t="inlineStr">
         <is>
@@ -3348,7 +3348,7 @@
         </is>
       </c>
       <c r="O45" t="n">
-        <v>170</v>
+        <v>197</v>
       </c>
       <c r="P45" t="inlineStr">
         <is>
@@ -3414,7 +3414,7 @@
         </is>
       </c>
       <c r="O46" t="n">
-        <v>143</v>
+        <v>161</v>
       </c>
       <c r="P46" t="inlineStr">
         <is>
@@ -3480,7 +3480,7 @@
         </is>
       </c>
       <c r="O47" t="n">
-        <v>1546</v>
+        <v>1750</v>
       </c>
       <c r="P47" t="inlineStr">
         <is>
@@ -3546,7 +3546,7 @@
         </is>
       </c>
       <c r="O48" t="n">
-        <v>1526</v>
+        <v>1794</v>
       </c>
       <c r="P48" t="inlineStr">
         <is>
@@ -3612,7 +3612,7 @@
         </is>
       </c>
       <c r="O49" t="n">
-        <v>280</v>
+        <v>314</v>
       </c>
       <c r="P49" t="inlineStr">
         <is>
@@ -3678,7 +3678,7 @@
         </is>
       </c>
       <c r="O50" t="n">
-        <v>235</v>
+        <v>274</v>
       </c>
       <c r="P50" t="inlineStr">
         <is>
@@ -3744,7 +3744,7 @@
         </is>
       </c>
       <c r="O51" t="n">
-        <v>651</v>
+        <v>696</v>
       </c>
       <c r="P51" t="inlineStr">
         <is>
@@ -3810,7 +3810,7 @@
         </is>
       </c>
       <c r="O52" t="n">
-        <v>670</v>
+        <v>742</v>
       </c>
       <c r="P52" t="inlineStr">
         <is>
@@ -3876,7 +3876,7 @@
         </is>
       </c>
       <c r="O53" t="n">
-        <v>428</v>
+        <v>470</v>
       </c>
       <c r="P53" t="inlineStr">
         <is>
@@ -3942,7 +3942,7 @@
         </is>
       </c>
       <c r="O54" t="n">
-        <v>279</v>
+        <v>308</v>
       </c>
       <c r="P54" t="inlineStr">
         <is>
@@ -4008,7 +4008,7 @@
         </is>
       </c>
       <c r="O55" t="n">
-        <v>629</v>
+        <v>728</v>
       </c>
       <c r="P55" t="inlineStr">
         <is>
@@ -4074,7 +4074,7 @@
         </is>
       </c>
       <c r="O56" t="n">
-        <v>550</v>
+        <v>597</v>
       </c>
       <c r="P56" t="inlineStr">
         <is>
@@ -4140,7 +4140,7 @@
         </is>
       </c>
       <c r="O57" t="n">
-        <v>1365</v>
+        <v>1347</v>
       </c>
       <c r="P57" t="inlineStr">
         <is>
@@ -4206,7 +4206,7 @@
         </is>
       </c>
       <c r="O58" t="n">
-        <v>1576</v>
+        <v>1605</v>
       </c>
       <c r="P58" t="inlineStr">
         <is>

</xml_diff>